<commit_message>
chore: remove unused data_suhu.xlsx file
</commit_message>
<xml_diff>
--- a/Dashboard/data_suhu.xlsx
+++ b/Dashboard/data_suhu.xlsx
@@ -12,6 +12,116 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
+</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>